<commit_message>
Gilds added + Clean up + Unittests
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -632,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +721,7 @@
         <v>2</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -914,7 +914,9 @@
       <c r="A36" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="9"/>
+      <c r="B36" s="9">
+        <v>3</v>
+      </c>
       <c r="C36" s="7">
         <v>3</v>
       </c>
@@ -957,7 +959,7 @@
         <v>30</v>
       </c>
       <c r="B41" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C41" s="7">
         <v>5</v>
@@ -967,7 +969,9 @@
       <c r="A42" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B42" s="9"/>
+      <c r="B42" s="9">
+        <v>0</v>
+      </c>
       <c r="C42" s="7">
         <v>5</v>
       </c>
@@ -1007,7 +1011,9 @@
       <c r="A48" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B48" s="9"/>
+      <c r="B48" s="9">
+        <v>2</v>
+      </c>
       <c r="C48" s="7">
         <v>2</v>
       </c>
@@ -1016,7 +1022,9 @@
       <c r="A49" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B49" s="9"/>
+      <c r="B49" s="9">
+        <v>2</v>
+      </c>
       <c r="C49" s="7">
         <v>2</v>
       </c>
@@ -1025,7 +1033,9 @@
       <c r="A50" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B50" s="9"/>
+      <c r="B50" s="9">
+        <v>2</v>
+      </c>
       <c r="C50" s="7">
         <v>2</v>
       </c>
@@ -1034,7 +1044,9 @@
       <c r="A51" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B51" s="9"/>
+      <c r="B51" s="9">
+        <v>1</v>
+      </c>
       <c r="C51" s="7">
         <v>1</v>
       </c>
@@ -1043,7 +1055,9 @@
       <c r="A52" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B52" s="9"/>
+      <c r="B52" s="9">
+        <v>1</v>
+      </c>
       <c r="C52" s="7">
         <v>1</v>
       </c>
@@ -1054,7 +1068,7 @@
       </c>
       <c r="B54" s="2">
         <f>IF(MIN(B9:B14)=1,SUM(B21:B52),0)</f>
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="C54" s="2">
         <f>SUM(C21:C52)</f>

</xml_diff>

<commit_message>
UML Diagram + Protokoll + Datenbank file
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -622,7 +622,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -632,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,7 +959,7 @@
         <v>30</v>
       </c>
       <c r="B41" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C41" s="7">
         <v>5</v>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="B54" s="2">
         <f>IF(MIN(B9:B14)=1,SUM(B21:B52),0)</f>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C54" s="2">
         <f>SUM(C21:C52)</f>

</xml_diff>